<commit_message>
ändrat amazon rank script och lagt in i YMLfil
</commit_message>
<xml_diff>
--- a/data/fractal_rank_tracking.xlsx
+++ b/data/fractal_rank_tracking.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,67 +461,10 @@
         <v>45</v>
       </c>
       <c r="D2" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-11-29</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>15</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-11-29</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>17</v>
-      </c>
-      <c r="C4" t="n">
-        <v>45</v>
-      </c>
-      <c r="D4" t="n">
-        <v>31</v>
-      </c>
-      <c r="E4" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-11-29</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>17</v>
-      </c>
-      <c r="C5" t="n">
-        <v>45</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>